<commit_message>
Commit before sleep and before Oxford import
</commit_message>
<xml_diff>
--- a/Data/SAMPLE_LISTS.xlsx
+++ b/Data/SAMPLE_LISTS.xlsx
@@ -8,14 +8,18 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/timodaehler/Desktop/COVID19-DOMINANCE/Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5A553DF3-BD50-B841-BBAB-779E3625FBF9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A0F0B8D4-B8F3-D841-8CA4-193132937BBA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16000" activeTab="1" xr2:uid="{48B91D4D-CE82-EA40-88A5-59D4871D7E70}"/>
+    <workbookView xWindow="-38400" yWindow="0" windowWidth="38400" windowHeight="21600" activeTab="4" xr2:uid="{48B91D4D-CE82-EA40-88A5-59D4871D7E70}"/>
   </bookViews>
   <sheets>
     <sheet name="ISO_CODES" sheetId="1" r:id="rId1"/>
     <sheet name="SAMPLE_LISTS" sheetId="9" r:id="rId2"/>
     <sheet name="SAMPLE_LISTS_R" sheetId="6" r:id="rId3"/>
+    <sheet name="Intermediate" sheetId="10" r:id="rId4"/>
+    <sheet name="EMBI" sheetId="11" r:id="rId5"/>
+    <sheet name="EMBI2" sheetId="12" r:id="rId6"/>
+    <sheet name="LEMB" sheetId="13" r:id="rId7"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -35,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2137" uniqueCount="1005">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2851" uniqueCount="1058">
   <si>
     <t>English short name</t>
   </si>
@@ -3050,13 +3054,172 @@
   </si>
   <si>
     <t>EIKON</t>
+  </si>
+  <si>
+    <t>laender</t>
+  </si>
+  <si>
+    <t>Bahamas</t>
+  </si>
+  <si>
+    <t>Bolivia</t>
+  </si>
+  <si>
+    <t>British Indian Ocean Territory</t>
+  </si>
+  <si>
+    <t>British Virgin Islands</t>
+  </si>
+  <si>
+    <t>Brunei</t>
+  </si>
+  <si>
+    <t>Burma</t>
+  </si>
+  <si>
+    <t>Cayman Islands</t>
+  </si>
+  <si>
+    <t>Central African Republic</t>
+  </si>
+  <si>
+    <t>Cocos [Keeling] Islands</t>
+  </si>
+  <si>
+    <t>Comoros</t>
+  </si>
+  <si>
+    <t>Congo (Brazzaville)</t>
+  </si>
+  <si>
+    <t>Congo (Kinshasa)</t>
+  </si>
+  <si>
+    <t>Cook Islands</t>
+  </si>
+  <si>
+    <t>Cote d'Ivoire</t>
+  </si>
+  <si>
+    <t>Dominican Republic</t>
+  </si>
+  <si>
+    <t>Falkland Islands [Islas Malvinas]</t>
+  </si>
+  <si>
+    <t>Faroe Islands</t>
+  </si>
+  <si>
+    <t>French Southern Territories</t>
+  </si>
+  <si>
+    <t>Gambia</t>
+  </si>
+  <si>
+    <t>Gaza Strip</t>
+  </si>
+  <si>
+    <t>Holy See</t>
+  </si>
+  <si>
+    <t>Iran</t>
+  </si>
+  <si>
+    <t>Korea, South</t>
+  </si>
+  <si>
+    <t>Laos</t>
+  </si>
+  <si>
+    <t>Macau</t>
+  </si>
+  <si>
+    <t>Marshall Islands</t>
+  </si>
+  <si>
+    <t>Micronesia</t>
+  </si>
+  <si>
+    <t>Moldova</t>
+  </si>
+  <si>
+    <t>Netherlands</t>
+  </si>
+  <si>
+    <t>Netherlands Antilles</t>
+  </si>
+  <si>
+    <t>Niger</t>
+  </si>
+  <si>
+    <t>North Korea</t>
+  </si>
+  <si>
+    <t>Northern Mariana Islands</t>
+  </si>
+  <si>
+    <t>Palestinian Territories</t>
+  </si>
+  <si>
+    <t>Philippines</t>
+  </si>
+  <si>
+    <t>Pitcairn Islands</t>
+  </si>
+  <si>
+    <t>Russia</t>
+  </si>
+  <si>
+    <t>Saint Helena</t>
+  </si>
+  <si>
+    <t>Sudan</t>
+  </si>
+  <si>
+    <t>Syria</t>
+  </si>
+  <si>
+    <t>Taiwan*</t>
+  </si>
+  <si>
+    <t>Tanzania</t>
+  </si>
+  <si>
+    <t>Turks and Caicos Islands</t>
+  </si>
+  <si>
+    <t>U.S. Minor Outlying Islands</t>
+  </si>
+  <si>
+    <t>U.S. Virgin Islands</t>
+  </si>
+  <si>
+    <t>United Arab Emirates</t>
+  </si>
+  <si>
+    <t>United Kingdom</t>
+  </si>
+  <si>
+    <t>Venezuela</t>
+  </si>
+  <si>
+    <t>Vietnam</t>
+  </si>
+  <si>
+    <t>Western Sahara</t>
+  </si>
+  <si>
+    <t>available</t>
+  </si>
+  <si>
+    <t>Country</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -3068,6 +3231,14 @@
       <sz val="10"/>
       <name val="Lucida Console"/>
       <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -3139,7 +3310,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
@@ -3152,6 +3323,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -9256,8 +9430,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F8131F12-2570-9846-B7A5-5492D8112941}">
   <dimension ref="A1:S158"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8:D18"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F4" sqref="F4:F36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -13972,7 +14146,7 @@
   <dimension ref="A1:R156"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I26" sqref="I26"/>
+      <selection activeCell="C2" sqref="C2:C20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -19228,4 +19402,3229 @@
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5AFDC7DB-2BD2-B747-993F-668F96434B9C}">
+  <dimension ref="D17:M263"/>
+  <sheetViews>
+    <sheetView topLeftCell="A52" workbookViewId="0">
+      <selection activeCell="G101" sqref="G101"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="4" max="4" width="40" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="17" spans="4:13" x14ac:dyDescent="0.2">
+      <c r="D17" s="12" t="s">
+        <v>1005</v>
+      </c>
+    </row>
+    <row r="18" spans="4:13" x14ac:dyDescent="0.2">
+      <c r="D18" t="s">
+        <v>13</v>
+      </c>
+      <c r="E18" t="s">
+        <v>1056</v>
+      </c>
+      <c r="H18" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="I18" t="str">
+        <f>VLOOKUP(H18,$D$18:$E$263,2,FALSE)</f>
+        <v>available</v>
+      </c>
+      <c r="L18" t="s">
+        <v>122</v>
+      </c>
+      <c r="M18" t="s">
+        <v>1056</v>
+      </c>
+    </row>
+    <row r="19" spans="4:13" x14ac:dyDescent="0.2">
+      <c r="D19" t="s">
+        <v>24</v>
+      </c>
+      <c r="E19" t="s">
+        <v>1056</v>
+      </c>
+      <c r="H19" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="I19" t="str">
+        <f t="shared" ref="I19:I68" si="0">VLOOKUP(H19,$D$18:$E$263,2,FALSE)</f>
+        <v>available</v>
+      </c>
+      <c r="L19" t="s">
+        <v>182</v>
+      </c>
+      <c r="M19" t="s">
+        <v>1056</v>
+      </c>
+    </row>
+    <row r="20" spans="4:13" x14ac:dyDescent="0.2">
+      <c r="D20" t="s">
+        <v>242</v>
+      </c>
+      <c r="E20" t="s">
+        <v>1056</v>
+      </c>
+      <c r="H20" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="I20" t="str">
+        <f t="shared" si="0"/>
+        <v>available</v>
+      </c>
+      <c r="L20" t="s">
+        <v>190</v>
+      </c>
+      <c r="M20" t="s">
+        <v>1056</v>
+      </c>
+    </row>
+    <row r="21" spans="4:13" x14ac:dyDescent="0.2">
+      <c r="D21" t="s">
+        <v>44</v>
+      </c>
+      <c r="E21" t="s">
+        <v>1056</v>
+      </c>
+      <c r="H21" s="2" t="s">
+        <v>122</v>
+      </c>
+      <c r="I21" t="str">
+        <f t="shared" si="0"/>
+        <v>available</v>
+      </c>
+      <c r="L21" t="s">
+        <v>194</v>
+      </c>
+      <c r="M21" t="s">
+        <v>1056</v>
+      </c>
+    </row>
+    <row r="22" spans="4:13" x14ac:dyDescent="0.2">
+      <c r="D22" t="s">
+        <v>5</v>
+      </c>
+      <c r="E22" t="s">
+        <v>1056</v>
+      </c>
+      <c r="H22" s="2" t="s">
+        <v>182</v>
+      </c>
+      <c r="I22" t="str">
+        <f t="shared" si="0"/>
+        <v>available</v>
+      </c>
+      <c r="L22" t="s">
+        <v>219</v>
+      </c>
+      <c r="M22" t="s">
+        <v>1056</v>
+      </c>
+    </row>
+    <row r="23" spans="4:13" x14ac:dyDescent="0.2">
+      <c r="D23" t="s">
+        <v>32</v>
+      </c>
+      <c r="E23" t="s">
+        <v>1056</v>
+      </c>
+      <c r="H23" s="2" t="s">
+        <v>190</v>
+      </c>
+      <c r="I23" t="str">
+        <f t="shared" si="0"/>
+        <v>available</v>
+      </c>
+      <c r="K23" t="s">
+        <v>238</v>
+      </c>
+      <c r="L23" t="s">
+        <v>1020</v>
+      </c>
+      <c r="M23" t="s">
+        <v>1056</v>
+      </c>
+    </row>
+    <row r="24" spans="4:13" x14ac:dyDescent="0.2">
+      <c r="D24" t="s">
+        <v>21</v>
+      </c>
+      <c r="E24" t="s">
+        <v>1056</v>
+      </c>
+      <c r="H24" s="2" t="s">
+        <v>194</v>
+      </c>
+      <c r="I24" t="str">
+        <f t="shared" si="0"/>
+        <v>available</v>
+      </c>
+      <c r="L24" t="s">
+        <v>391</v>
+      </c>
+      <c r="M24" t="s">
+        <v>1056</v>
+      </c>
+    </row>
+    <row r="25" spans="4:13" x14ac:dyDescent="0.2">
+      <c r="D25" t="s">
+        <v>36</v>
+      </c>
+      <c r="E25" t="s">
+        <v>1056</v>
+      </c>
+      <c r="G25" s="2" t="s">
+        <v>238</v>
+      </c>
+      <c r="H25" s="2" t="s">
+        <v>1020</v>
+      </c>
+      <c r="I25" t="str">
+        <f t="shared" si="0"/>
+        <v>available</v>
+      </c>
+      <c r="L25" t="s">
+        <v>395</v>
+      </c>
+      <c r="M25" t="s">
+        <v>1056</v>
+      </c>
+    </row>
+    <row r="26" spans="4:13" x14ac:dyDescent="0.2">
+      <c r="D26" t="s">
+        <v>17</v>
+      </c>
+      <c r="E26" t="s">
+        <v>1056</v>
+      </c>
+      <c r="H26" s="2" t="s">
+        <v>254</v>
+      </c>
+      <c r="I26" t="str">
+        <f t="shared" si="0"/>
+        <v>available</v>
+      </c>
+      <c r="L26" t="s">
+        <v>612</v>
+      </c>
+      <c r="M26" t="s">
+        <v>1056</v>
+      </c>
+    </row>
+    <row r="27" spans="4:13" x14ac:dyDescent="0.2">
+      <c r="D27" t="s">
+        <v>40</v>
+      </c>
+      <c r="E27" t="s">
+        <v>1056</v>
+      </c>
+      <c r="H27" s="2" t="s">
+        <v>322</v>
+      </c>
+      <c r="I27" t="str">
+        <f t="shared" si="0"/>
+        <v>available</v>
+      </c>
+      <c r="L27" t="s">
+        <v>616</v>
+      </c>
+      <c r="M27" t="s">
+        <v>1056</v>
+      </c>
+    </row>
+    <row r="28" spans="4:13" x14ac:dyDescent="0.2">
+      <c r="D28" t="s">
+        <v>28</v>
+      </c>
+      <c r="E28" t="s">
+        <v>1056</v>
+      </c>
+      <c r="H28" s="2" t="s">
+        <v>391</v>
+      </c>
+      <c r="I28" t="str">
+        <f t="shared" si="0"/>
+        <v>available</v>
+      </c>
+      <c r="L28" t="s">
+        <v>677</v>
+      </c>
+      <c r="M28" t="s">
+        <v>1056</v>
+      </c>
+    </row>
+    <row r="29" spans="4:13" x14ac:dyDescent="0.2">
+      <c r="D29" t="s">
+        <v>56</v>
+      </c>
+      <c r="E29" t="s">
+        <v>1056</v>
+      </c>
+      <c r="H29" s="2" t="s">
+        <v>395</v>
+      </c>
+      <c r="I29" t="str">
+        <f t="shared" si="0"/>
+        <v>available</v>
+      </c>
+      <c r="K29" t="s">
+        <v>689</v>
+      </c>
+      <c r="L29" t="s">
+        <v>1040</v>
+      </c>
+      <c r="M29" t="s">
+        <v>1056</v>
+      </c>
+    </row>
+    <row r="30" spans="4:13" x14ac:dyDescent="0.2">
+      <c r="D30" t="s">
+        <v>52</v>
+      </c>
+      <c r="E30" t="s">
+        <v>1056</v>
+      </c>
+      <c r="H30" s="2" t="s">
+        <v>489</v>
+      </c>
+      <c r="I30" t="str">
+        <f t="shared" si="0"/>
+        <v>available</v>
+      </c>
+      <c r="L30" t="s">
+        <v>697</v>
+      </c>
+      <c r="M30" t="s">
+        <v>1056</v>
+      </c>
+    </row>
+    <row r="31" spans="4:13" x14ac:dyDescent="0.2">
+      <c r="D31" t="s">
+        <v>48</v>
+      </c>
+      <c r="E31" t="s">
+        <v>1056</v>
+      </c>
+      <c r="H31" s="2" t="s">
+        <v>616</v>
+      </c>
+      <c r="I31" t="str">
+        <f t="shared" si="0"/>
+        <v>available</v>
+      </c>
+      <c r="L31" t="s">
+        <v>736</v>
+      </c>
+      <c r="M31" t="s">
+        <v>1056</v>
+      </c>
+    </row>
+    <row r="32" spans="4:13" x14ac:dyDescent="0.2">
+      <c r="D32" t="s">
+        <v>63</v>
+      </c>
+      <c r="E32" t="s">
+        <v>1056</v>
+      </c>
+      <c r="H32" s="2" t="s">
+        <v>612</v>
+      </c>
+      <c r="I32" t="str">
+        <f t="shared" si="0"/>
+        <v>available</v>
+      </c>
+      <c r="K32" t="s">
+        <v>744</v>
+      </c>
+      <c r="L32" t="s">
+        <v>1042</v>
+      </c>
+      <c r="M32" t="s">
+        <v>1056</v>
+      </c>
+    </row>
+    <row r="33" spans="4:13" x14ac:dyDescent="0.2">
+      <c r="D33" t="s">
+        <v>1006</v>
+      </c>
+      <c r="E33" t="s">
+        <v>1056</v>
+      </c>
+      <c r="H33" s="2" t="s">
+        <v>640</v>
+      </c>
+      <c r="I33" t="str">
+        <f t="shared" si="0"/>
+        <v>available</v>
+      </c>
+      <c r="L33" t="s">
+        <v>851</v>
+      </c>
+      <c r="M33" t="s">
+        <v>1056</v>
+      </c>
+    </row>
+    <row r="34" spans="4:13" x14ac:dyDescent="0.2">
+      <c r="D34" t="s">
+        <v>91</v>
+      </c>
+      <c r="E34" t="s">
+        <v>1056</v>
+      </c>
+      <c r="H34" s="2" t="s">
+        <v>670</v>
+      </c>
+      <c r="I34" t="str">
+        <f t="shared" si="0"/>
+        <v>available</v>
+      </c>
+      <c r="L34" t="s">
+        <v>879</v>
+      </c>
+      <c r="M34" t="s">
+        <v>1056</v>
+      </c>
+    </row>
+    <row r="35" spans="4:13" x14ac:dyDescent="0.2">
+      <c r="D35" t="s">
+        <v>75</v>
+      </c>
+      <c r="E35" t="s">
+        <v>1056</v>
+      </c>
+      <c r="H35" s="2" t="s">
+        <v>673</v>
+      </c>
+      <c r="I35" t="str">
+        <f t="shared" si="0"/>
+        <v>available</v>
+      </c>
+      <c r="L35" t="s">
+        <v>915</v>
+      </c>
+      <c r="M35" t="s">
+        <v>1056</v>
+      </c>
+    </row>
+    <row r="36" spans="4:13" x14ac:dyDescent="0.2">
+      <c r="D36" t="s">
+        <v>71</v>
+      </c>
+      <c r="E36" t="s">
+        <v>1056</v>
+      </c>
+      <c r="H36" s="2" t="s">
+        <v>677</v>
+      </c>
+      <c r="I36" t="str">
+        <f t="shared" si="0"/>
+        <v>available</v>
+      </c>
+      <c r="L36" t="s">
+        <v>966</v>
+      </c>
+      <c r="M36" t="s">
+        <v>1056</v>
+      </c>
+    </row>
+    <row r="37" spans="4:13" x14ac:dyDescent="0.2">
+      <c r="D37" t="s">
+        <v>142</v>
+      </c>
+      <c r="E37" t="s">
+        <v>1056</v>
+      </c>
+      <c r="G37" s="2" t="s">
+        <v>689</v>
+      </c>
+      <c r="H37" s="2" t="s">
+        <v>1040</v>
+      </c>
+      <c r="I37" t="str">
+        <f t="shared" si="0"/>
+        <v>available</v>
+      </c>
+    </row>
+    <row r="38" spans="4:13" x14ac:dyDescent="0.2">
+      <c r="D38" t="s">
+        <v>79</v>
+      </c>
+      <c r="E38" t="s">
+        <v>1056</v>
+      </c>
+      <c r="H38" s="2" t="s">
+        <v>697</v>
+      </c>
+      <c r="I38" t="str">
+        <f t="shared" si="0"/>
+        <v>available</v>
+      </c>
+    </row>
+    <row r="39" spans="4:13" x14ac:dyDescent="0.2">
+      <c r="D39" t="s">
+        <v>146</v>
+      </c>
+      <c r="E39" t="s">
+        <v>1056</v>
+      </c>
+      <c r="H39" s="2" t="s">
+        <v>728</v>
+      </c>
+      <c r="I39" t="str">
+        <f t="shared" si="0"/>
+        <v>available</v>
+      </c>
+    </row>
+    <row r="40" spans="4:13" x14ac:dyDescent="0.2">
+      <c r="D40" t="s">
+        <v>99</v>
+      </c>
+      <c r="E40" t="s">
+        <v>1056</v>
+      </c>
+      <c r="H40" s="2" t="s">
+        <v>736</v>
+      </c>
+      <c r="I40" t="str">
+        <f t="shared" si="0"/>
+        <v>available</v>
+      </c>
+    </row>
+    <row r="41" spans="4:13" x14ac:dyDescent="0.2">
+      <c r="D41" t="s">
+        <v>106</v>
+      </c>
+      <c r="E41" t="s">
+        <v>1056</v>
+      </c>
+      <c r="G41" s="2" t="s">
+        <v>744</v>
+      </c>
+      <c r="H41" s="2" t="s">
+        <v>1042</v>
+      </c>
+      <c r="I41" t="str">
+        <f t="shared" si="0"/>
+        <v>available</v>
+      </c>
+    </row>
+    <row r="42" spans="4:13" x14ac:dyDescent="0.2">
+      <c r="D42" t="s">
+        <v>130</v>
+      </c>
+      <c r="E42" t="s">
+        <v>1056</v>
+      </c>
+      <c r="H42" s="2" t="s">
+        <v>752</v>
+      </c>
+      <c r="I42" t="str">
+        <f t="shared" si="0"/>
+        <v>available</v>
+      </c>
+    </row>
+    <row r="43" spans="4:13" x14ac:dyDescent="0.2">
+      <c r="D43" t="s">
+        <v>1007</v>
+      </c>
+      <c r="E43" t="s">
+        <v>1056</v>
+      </c>
+      <c r="H43" s="2" t="s">
+        <v>966</v>
+      </c>
+      <c r="I43" t="str">
+        <f t="shared" si="0"/>
+        <v>available</v>
+      </c>
+    </row>
+    <row r="44" spans="4:13" x14ac:dyDescent="0.2">
+      <c r="D44" t="s">
+        <v>67</v>
+      </c>
+      <c r="E44" t="s">
+        <v>1056</v>
+      </c>
+      <c r="H44" s="2" t="s">
+        <v>509</v>
+      </c>
+      <c r="I44" t="str">
+        <f t="shared" si="0"/>
+        <v>available</v>
+      </c>
+    </row>
+    <row r="45" spans="4:13" x14ac:dyDescent="0.2">
+      <c r="D45" t="s">
+        <v>138</v>
+      </c>
+      <c r="E45" t="s">
+        <v>1056</v>
+      </c>
+      <c r="H45" s="2" t="s">
+        <v>879</v>
+      </c>
+      <c r="I45" t="str">
+        <f t="shared" si="0"/>
+        <v>available</v>
+      </c>
+    </row>
+    <row r="46" spans="4:13" x14ac:dyDescent="0.2">
+      <c r="D46" t="s">
+        <v>134</v>
+      </c>
+      <c r="E46" t="s">
+        <v>1056</v>
+      </c>
+      <c r="H46" s="2" t="s">
+        <v>899</v>
+      </c>
+      <c r="I46" t="str">
+        <f t="shared" si="0"/>
+        <v>available</v>
+      </c>
+    </row>
+    <row r="47" spans="4:13" x14ac:dyDescent="0.2">
+      <c r="D47" t="s">
+        <v>122</v>
+      </c>
+      <c r="E47" t="s">
+        <v>1056</v>
+      </c>
+      <c r="G47" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="H47" s="2" t="s">
+        <v>1051</v>
+      </c>
+      <c r="I47" t="str">
+        <f t="shared" si="0"/>
+        <v>available</v>
+      </c>
+    </row>
+    <row r="48" spans="4:13" x14ac:dyDescent="0.2">
+      <c r="D48" t="s">
+        <v>1008</v>
+      </c>
+      <c r="E48" t="s">
+        <v>1056</v>
+      </c>
+      <c r="H48" s="2" t="s">
+        <v>915</v>
+      </c>
+      <c r="I48" t="str">
+        <f t="shared" si="0"/>
+        <v>available</v>
+      </c>
+    </row>
+    <row r="49" spans="4:9" x14ac:dyDescent="0.2">
+      <c r="D49" t="s">
+        <v>1009</v>
+      </c>
+      <c r="E49" t="s">
+        <v>1056</v>
+      </c>
+    </row>
+    <row r="50" spans="4:9" x14ac:dyDescent="0.2">
+      <c r="D50" t="s">
+        <v>1010</v>
+      </c>
+      <c r="E50" t="s">
+        <v>1056</v>
+      </c>
+      <c r="G50" s="2"/>
+      <c r="H50" s="2" t="s">
+        <v>122</v>
+      </c>
+      <c r="I50" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>available</v>
+      </c>
+    </row>
+    <row r="51" spans="4:9" x14ac:dyDescent="0.2">
+      <c r="D51" t="s">
+        <v>87</v>
+      </c>
+      <c r="E51" t="s">
+        <v>1056</v>
+      </c>
+      <c r="G51" s="2"/>
+      <c r="H51" s="2" t="s">
+        <v>182</v>
+      </c>
+      <c r="I51" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>available</v>
+      </c>
+    </row>
+    <row r="52" spans="4:9" x14ac:dyDescent="0.2">
+      <c r="D52" t="s">
+        <v>83</v>
+      </c>
+      <c r="E52" t="s">
+        <v>1056</v>
+      </c>
+      <c r="G52" s="2"/>
+      <c r="H52" s="2" t="s">
+        <v>190</v>
+      </c>
+      <c r="I52" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>available</v>
+      </c>
+    </row>
+    <row r="53" spans="4:9" x14ac:dyDescent="0.2">
+      <c r="D53" t="s">
+        <v>1011</v>
+      </c>
+      <c r="E53" t="s">
+        <v>1056</v>
+      </c>
+      <c r="G53" s="2"/>
+      <c r="H53" s="2" t="s">
+        <v>194</v>
+      </c>
+      <c r="I53" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>available</v>
+      </c>
+    </row>
+    <row r="54" spans="4:9" x14ac:dyDescent="0.2">
+      <c r="D54" t="s">
+        <v>95</v>
+      </c>
+      <c r="E54" t="s">
+        <v>1056</v>
+      </c>
+      <c r="G54" s="2"/>
+      <c r="H54" s="2" t="s">
+        <v>219</v>
+      </c>
+      <c r="I54" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>available</v>
+      </c>
+    </row>
+    <row r="55" spans="4:9" x14ac:dyDescent="0.2">
+      <c r="D55" t="s">
+        <v>205</v>
+      </c>
+      <c r="E55" t="s">
+        <v>1056</v>
+      </c>
+      <c r="G55" s="2" t="s">
+        <v>238</v>
+      </c>
+      <c r="H55" s="2" t="s">
+        <v>1020</v>
+      </c>
+      <c r="I55" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>available</v>
+      </c>
+    </row>
+    <row r="56" spans="4:9" x14ac:dyDescent="0.2">
+      <c r="D56" t="s">
+        <v>458</v>
+      </c>
+      <c r="E56" t="s">
+        <v>1056</v>
+      </c>
+      <c r="G56" s="2"/>
+      <c r="H56" s="2" t="s">
+        <v>391</v>
+      </c>
+      <c r="I56" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>available</v>
+      </c>
+    </row>
+    <row r="57" spans="4:9" x14ac:dyDescent="0.2">
+      <c r="D57" t="s">
+        <v>186</v>
+      </c>
+      <c r="E57" t="s">
+        <v>1056</v>
+      </c>
+      <c r="G57" s="2"/>
+      <c r="H57" s="2" t="s">
+        <v>395</v>
+      </c>
+      <c r="I57" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>available</v>
+      </c>
+    </row>
+    <row r="58" spans="4:9" x14ac:dyDescent="0.2">
+      <c r="D58" t="s">
+        <v>150</v>
+      </c>
+      <c r="E58" t="s">
+        <v>1056</v>
+      </c>
+      <c r="G58" s="2"/>
+      <c r="H58" s="2" t="s">
+        <v>612</v>
+      </c>
+      <c r="I58" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>available</v>
+      </c>
+    </row>
+    <row r="59" spans="4:9" x14ac:dyDescent="0.2">
+      <c r="D59" t="s">
+        <v>1012</v>
+      </c>
+      <c r="E59" t="s">
+        <v>1056</v>
+      </c>
+      <c r="G59" s="2"/>
+      <c r="H59" s="2" t="s">
+        <v>616</v>
+      </c>
+      <c r="I59" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>available</v>
+      </c>
+    </row>
+    <row r="60" spans="4:9" x14ac:dyDescent="0.2">
+      <c r="D60" t="s">
+        <v>1013</v>
+      </c>
+      <c r="E60" t="s">
+        <v>1056</v>
+      </c>
+      <c r="G60" s="2"/>
+      <c r="H60" s="2" t="s">
+        <v>677</v>
+      </c>
+      <c r="I60" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>available</v>
+      </c>
+    </row>
+    <row r="61" spans="4:9" x14ac:dyDescent="0.2">
+      <c r="D61" t="s">
+        <v>839</v>
+      </c>
+      <c r="E61" t="s">
+        <v>1056</v>
+      </c>
+      <c r="G61" s="2" t="s">
+        <v>689</v>
+      </c>
+      <c r="H61" s="2" t="s">
+        <v>1040</v>
+      </c>
+      <c r="I61" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>available</v>
+      </c>
+    </row>
+    <row r="62" spans="4:9" x14ac:dyDescent="0.2">
+      <c r="D62" t="s">
+        <v>182</v>
+      </c>
+      <c r="E62" t="s">
+        <v>1056</v>
+      </c>
+      <c r="G62" s="2"/>
+      <c r="H62" s="2" t="s">
+        <v>697</v>
+      </c>
+      <c r="I62" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>available</v>
+      </c>
+    </row>
+    <row r="63" spans="4:9" x14ac:dyDescent="0.2">
+      <c r="D63" t="s">
+        <v>190</v>
+      </c>
+      <c r="E63" t="s">
+        <v>1056</v>
+      </c>
+      <c r="G63" s="2"/>
+      <c r="H63" s="2" t="s">
+        <v>736</v>
+      </c>
+      <c r="I63" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>available</v>
+      </c>
+    </row>
+    <row r="64" spans="4:9" x14ac:dyDescent="0.2">
+      <c r="D64" t="s">
+        <v>211</v>
+      </c>
+      <c r="E64" t="s">
+        <v>1056</v>
+      </c>
+      <c r="G64" s="2" t="s">
+        <v>744</v>
+      </c>
+      <c r="H64" s="2" t="s">
+        <v>1042</v>
+      </c>
+      <c r="I64" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>available</v>
+      </c>
+    </row>
+    <row r="65" spans="4:9" x14ac:dyDescent="0.2">
+      <c r="D65" t="s">
+        <v>1014</v>
+      </c>
+      <c r="E65" t="s">
+        <v>1056</v>
+      </c>
+      <c r="G65" s="2"/>
+      <c r="H65" s="2" t="s">
+        <v>851</v>
+      </c>
+      <c r="I65" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>available</v>
+      </c>
+    </row>
+    <row r="66" spans="4:9" x14ac:dyDescent="0.2">
+      <c r="D66" t="s">
+        <v>194</v>
+      </c>
+      <c r="E66" t="s">
+        <v>1056</v>
+      </c>
+      <c r="G66" s="2"/>
+      <c r="H66" s="2" t="s">
+        <v>879</v>
+      </c>
+      <c r="I66" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>available</v>
+      </c>
+    </row>
+    <row r="67" spans="4:9" x14ac:dyDescent="0.2">
+      <c r="D67" t="s">
+        <v>1015</v>
+      </c>
+      <c r="E67" t="s">
+        <v>1056</v>
+      </c>
+      <c r="G67" s="2"/>
+      <c r="H67" s="2" t="s">
+        <v>915</v>
+      </c>
+      <c r="I67" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>available</v>
+      </c>
+    </row>
+    <row r="68" spans="4:9" x14ac:dyDescent="0.2">
+      <c r="D68" t="s">
+        <v>1016</v>
+      </c>
+      <c r="E68" t="s">
+        <v>1056</v>
+      </c>
+      <c r="G68" s="2"/>
+      <c r="H68" s="2" t="s">
+        <v>966</v>
+      </c>
+      <c r="I68" s="2" t="str">
+        <f>VLOOKUP(H68,$D$18:$E$263,2,FALSE)</f>
+        <v>available</v>
+      </c>
+    </row>
+    <row r="69" spans="4:9" x14ac:dyDescent="0.2">
+      <c r="D69" t="s">
+        <v>1017</v>
+      </c>
+      <c r="E69" t="s">
+        <v>1056</v>
+      </c>
+      <c r="I69" s="2"/>
+    </row>
+    <row r="70" spans="4:9" x14ac:dyDescent="0.2">
+      <c r="D70" t="s">
+        <v>1018</v>
+      </c>
+      <c r="E70" t="s">
+        <v>1056</v>
+      </c>
+      <c r="F70" s="2"/>
+      <c r="G70" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="H70" s="2" t="s">
+        <v>1051</v>
+      </c>
+      <c r="I70" s="2" t="str">
+        <f t="shared" ref="I69:I102" si="1">VLOOKUP(H70,$D$18:$E$263,2,FALSE)</f>
+        <v>available</v>
+      </c>
+    </row>
+    <row r="71" spans="4:9" x14ac:dyDescent="0.2">
+      <c r="D71" t="s">
+        <v>198</v>
+      </c>
+      <c r="E71" t="s">
+        <v>1056</v>
+      </c>
+      <c r="H71" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="I71" s="2" t="str">
+        <f t="shared" si="1"/>
+        <v>available</v>
+      </c>
+    </row>
+    <row r="72" spans="4:9" x14ac:dyDescent="0.2">
+      <c r="D72" t="s">
+        <v>1019</v>
+      </c>
+      <c r="E72" t="s">
+        <v>1056</v>
+      </c>
+      <c r="H72" s="6" t="s">
+        <v>63</v>
+      </c>
+      <c r="I72" s="2" t="str">
+        <f t="shared" si="1"/>
+        <v>available</v>
+      </c>
+    </row>
+    <row r="73" spans="4:9" x14ac:dyDescent="0.2">
+      <c r="D73" t="s">
+        <v>383</v>
+      </c>
+      <c r="E73" t="s">
+        <v>1056</v>
+      </c>
+      <c r="H73" s="6" t="s">
+        <v>91</v>
+      </c>
+      <c r="I73" s="2" t="str">
+        <f t="shared" si="1"/>
+        <v>available</v>
+      </c>
+    </row>
+    <row r="74" spans="4:9" x14ac:dyDescent="0.2">
+      <c r="D74" t="s">
+        <v>202</v>
+      </c>
+      <c r="E74" t="s">
+        <v>1056</v>
+      </c>
+      <c r="H74" s="6" t="s">
+        <v>122</v>
+      </c>
+      <c r="I74" s="2" t="str">
+        <f t="shared" si="1"/>
+        <v>available</v>
+      </c>
+    </row>
+    <row r="75" spans="4:9" x14ac:dyDescent="0.2">
+      <c r="D75" t="s">
+        <v>215</v>
+      </c>
+      <c r="E75" t="s">
+        <v>1056</v>
+      </c>
+      <c r="H75" s="6" t="s">
+        <v>182</v>
+      </c>
+      <c r="I75" s="2" t="str">
+        <f t="shared" si="1"/>
+        <v>available</v>
+      </c>
+    </row>
+    <row r="76" spans="4:9" x14ac:dyDescent="0.2">
+      <c r="D76" t="s">
+        <v>219</v>
+      </c>
+      <c r="E76" t="s">
+        <v>1056</v>
+      </c>
+      <c r="H76" s="6" t="s">
+        <v>190</v>
+      </c>
+      <c r="I76" s="2" t="str">
+        <f t="shared" si="1"/>
+        <v>available</v>
+      </c>
+    </row>
+    <row r="77" spans="4:9" x14ac:dyDescent="0.2">
+      <c r="D77" t="s">
+        <v>230</v>
+      </c>
+      <c r="E77" t="s">
+        <v>1056</v>
+      </c>
+      <c r="H77" s="6" t="s">
+        <v>194</v>
+      </c>
+      <c r="I77" s="2" t="str">
+        <f t="shared" si="1"/>
+        <v>available</v>
+      </c>
+    </row>
+    <row r="78" spans="4:9" x14ac:dyDescent="0.2">
+      <c r="D78" t="s">
+        <v>227</v>
+      </c>
+      <c r="E78" t="s">
+        <v>1056</v>
+      </c>
+      <c r="G78" s="6" t="s">
+        <v>238</v>
+      </c>
+      <c r="H78" s="6" t="s">
+        <v>1020</v>
+      </c>
+      <c r="I78" s="2" t="str">
+        <f t="shared" si="1"/>
+        <v>available</v>
+      </c>
+    </row>
+    <row r="79" spans="4:9" x14ac:dyDescent="0.2">
+      <c r="D79" t="s">
+        <v>234</v>
+      </c>
+      <c r="E79" t="s">
+        <v>1056</v>
+      </c>
+      <c r="H79" s="6" t="s">
+        <v>254</v>
+      </c>
+      <c r="I79" s="2" t="str">
+        <f t="shared" si="1"/>
+        <v>available</v>
+      </c>
+    </row>
+    <row r="80" spans="4:9" x14ac:dyDescent="0.2">
+      <c r="D80" t="s">
+        <v>1020</v>
+      </c>
+      <c r="E80" t="s">
+        <v>1056</v>
+      </c>
+      <c r="H80" s="6" t="s">
+        <v>322</v>
+      </c>
+      <c r="I80" s="2" t="str">
+        <f t="shared" si="1"/>
+        <v>available</v>
+      </c>
+    </row>
+    <row r="81" spans="4:9" x14ac:dyDescent="0.2">
+      <c r="D81" t="s">
+        <v>246</v>
+      </c>
+      <c r="E81" t="s">
+        <v>1056</v>
+      </c>
+      <c r="H81" s="6" t="s">
+        <v>391</v>
+      </c>
+      <c r="I81" s="2" t="str">
+        <f t="shared" si="1"/>
+        <v>available</v>
+      </c>
+    </row>
+    <row r="82" spans="4:9" x14ac:dyDescent="0.2">
+      <c r="D82" t="s">
+        <v>254</v>
+      </c>
+      <c r="E82" t="s">
+        <v>1056</v>
+      </c>
+      <c r="H82" s="6" t="s">
+        <v>395</v>
+      </c>
+      <c r="I82" s="2" t="str">
+        <f t="shared" si="1"/>
+        <v>available</v>
+      </c>
+    </row>
+    <row r="83" spans="4:9" x14ac:dyDescent="0.2">
+      <c r="D83" t="s">
+        <v>820</v>
+      </c>
+      <c r="E83" t="s">
+        <v>1056</v>
+      </c>
+      <c r="H83" s="6" t="s">
+        <v>411</v>
+      </c>
+      <c r="I83" s="2" t="str">
+        <f t="shared" si="1"/>
+        <v>available</v>
+      </c>
+    </row>
+    <row r="84" spans="4:9" x14ac:dyDescent="0.2">
+      <c r="D84" t="s">
+        <v>345</v>
+      </c>
+      <c r="E84" t="s">
+        <v>1056</v>
+      </c>
+      <c r="H84" s="6" t="s">
+        <v>489</v>
+      </c>
+      <c r="I84" s="2" t="str">
+        <f t="shared" si="1"/>
+        <v>available</v>
+      </c>
+    </row>
+    <row r="85" spans="4:9" x14ac:dyDescent="0.2">
+      <c r="D85" t="s">
+        <v>262</v>
+      </c>
+      <c r="E85" t="s">
+        <v>1056</v>
+      </c>
+      <c r="H85" s="6" t="s">
+        <v>509</v>
+      </c>
+      <c r="I85" s="2" t="str">
+        <f t="shared" si="1"/>
+        <v>available</v>
+      </c>
+    </row>
+    <row r="86" spans="4:9" x14ac:dyDescent="0.2">
+      <c r="D86" t="s">
+        <v>250</v>
+      </c>
+      <c r="E86" t="s">
+        <v>1056</v>
+      </c>
+      <c r="H86" s="6" t="s">
+        <v>612</v>
+      </c>
+      <c r="I86" s="2" t="str">
+        <f t="shared" si="1"/>
+        <v>available</v>
+      </c>
+    </row>
+    <row r="87" spans="4:9" x14ac:dyDescent="0.2">
+      <c r="D87" t="s">
+        <v>831</v>
+      </c>
+      <c r="E87" t="s">
+        <v>1056</v>
+      </c>
+      <c r="H87" s="6" t="s">
+        <v>616</v>
+      </c>
+      <c r="I87" s="2" t="str">
+        <f t="shared" si="1"/>
+        <v>available</v>
+      </c>
+    </row>
+    <row r="88" spans="4:9" x14ac:dyDescent="0.2">
+      <c r="D88" t="s">
+        <v>270</v>
+      </c>
+      <c r="E88" t="s">
+        <v>1056</v>
+      </c>
+      <c r="H88" s="6" t="s">
+        <v>640</v>
+      </c>
+      <c r="I88" s="2" t="str">
+        <f t="shared" si="1"/>
+        <v>available</v>
+      </c>
+    </row>
+    <row r="89" spans="4:9" x14ac:dyDescent="0.2">
+      <c r="D89" t="s">
+        <v>1021</v>
+      </c>
+      <c r="E89" t="s">
+        <v>1056</v>
+      </c>
+      <c r="H89" s="6" t="s">
+        <v>670</v>
+      </c>
+      <c r="I89" s="2" t="str">
+        <f t="shared" si="1"/>
+        <v>available</v>
+      </c>
+    </row>
+    <row r="90" spans="4:9" x14ac:dyDescent="0.2">
+      <c r="D90" t="s">
+        <v>1022</v>
+      </c>
+      <c r="E90" t="s">
+        <v>1056</v>
+      </c>
+      <c r="H90" s="6" t="s">
+        <v>673</v>
+      </c>
+      <c r="I90" s="2" t="str">
+        <f t="shared" si="1"/>
+        <v>available</v>
+      </c>
+    </row>
+    <row r="91" spans="4:9" x14ac:dyDescent="0.2">
+      <c r="D91" t="s">
+        <v>278</v>
+      </c>
+      <c r="E91" t="s">
+        <v>1056</v>
+      </c>
+      <c r="H91" s="6" t="s">
+        <v>677</v>
+      </c>
+      <c r="I91" s="2" t="str">
+        <f t="shared" si="1"/>
+        <v>available</v>
+      </c>
+    </row>
+    <row r="92" spans="4:9" x14ac:dyDescent="0.2">
+      <c r="D92" t="s">
+        <v>274</v>
+      </c>
+      <c r="E92" t="s">
+        <v>1056</v>
+      </c>
+      <c r="G92" t="s">
+        <v>689</v>
+      </c>
+      <c r="H92" s="6" t="s">
+        <v>1040</v>
+      </c>
+      <c r="I92" s="2" t="str">
+        <f t="shared" si="1"/>
+        <v>available</v>
+      </c>
+    </row>
+    <row r="93" spans="4:9" x14ac:dyDescent="0.2">
+      <c r="D93" t="s">
+        <v>294</v>
+      </c>
+      <c r="E93" t="s">
+        <v>1056</v>
+      </c>
+      <c r="H93" s="6" t="s">
+        <v>697</v>
+      </c>
+      <c r="I93" s="2" t="str">
+        <f t="shared" si="1"/>
+        <v>available</v>
+      </c>
+    </row>
+    <row r="94" spans="4:9" x14ac:dyDescent="0.2">
+      <c r="D94" t="s">
+        <v>314</v>
+      </c>
+      <c r="E94" t="s">
+        <v>1056</v>
+      </c>
+      <c r="H94" s="6" t="s">
+        <v>728</v>
+      </c>
+      <c r="I94" s="2" t="str">
+        <f t="shared" si="1"/>
+        <v>available</v>
+      </c>
+    </row>
+    <row r="95" spans="4:9" x14ac:dyDescent="0.2">
+      <c r="D95" t="s">
+        <v>681</v>
+      </c>
+      <c r="E95" t="s">
+        <v>1056</v>
+      </c>
+      <c r="H95" s="6" t="s">
+        <v>736</v>
+      </c>
+      <c r="I95" s="2" t="str">
+        <f t="shared" si="1"/>
+        <v>available</v>
+      </c>
+    </row>
+    <row r="96" spans="4:9" x14ac:dyDescent="0.2">
+      <c r="D96" t="s">
+        <v>1023</v>
+      </c>
+      <c r="E96" t="s">
+        <v>1056</v>
+      </c>
+      <c r="G96" s="2" t="s">
+        <v>744</v>
+      </c>
+      <c r="H96" s="6" t="s">
+        <v>1042</v>
+      </c>
+      <c r="I96" s="2" t="str">
+        <f t="shared" si="1"/>
+        <v>available</v>
+      </c>
+    </row>
+    <row r="97" spans="4:9" x14ac:dyDescent="0.2">
+      <c r="D97" t="s">
+        <v>298</v>
+      </c>
+      <c r="E97" t="s">
+        <v>1056</v>
+      </c>
+      <c r="H97" s="6" t="s">
+        <v>752</v>
+      </c>
+      <c r="I97" s="2" t="str">
+        <f t="shared" si="1"/>
+        <v>available</v>
+      </c>
+    </row>
+    <row r="98" spans="4:9" x14ac:dyDescent="0.2">
+      <c r="D98" t="s">
+        <v>1024</v>
+      </c>
+      <c r="E98" t="s">
+        <v>1056</v>
+      </c>
+      <c r="H98" s="6" t="s">
+        <v>851</v>
+      </c>
+      <c r="I98" s="2" t="str">
+        <f t="shared" si="1"/>
+        <v>available</v>
+      </c>
+    </row>
+    <row r="99" spans="4:9" x14ac:dyDescent="0.2">
+      <c r="D99" t="s">
+        <v>1025</v>
+      </c>
+      <c r="E99" t="s">
+        <v>1056</v>
+      </c>
+      <c r="H99" s="6" t="s">
+        <v>879</v>
+      </c>
+      <c r="I99" s="2" t="str">
+        <f t="shared" si="1"/>
+        <v>available</v>
+      </c>
+    </row>
+    <row r="100" spans="4:9" x14ac:dyDescent="0.2">
+      <c r="D100" t="s">
+        <v>310</v>
+      </c>
+      <c r="E100" t="s">
+        <v>1056</v>
+      </c>
+      <c r="H100" s="6" t="s">
+        <v>899</v>
+      </c>
+      <c r="I100" s="2" t="str">
+        <f t="shared" si="1"/>
+        <v>available</v>
+      </c>
+    </row>
+    <row r="101" spans="4:9" x14ac:dyDescent="0.2">
+      <c r="D101" t="s">
+        <v>223</v>
+      </c>
+      <c r="E101" t="s">
+        <v>1056</v>
+      </c>
+      <c r="H101" s="6" t="s">
+        <v>915</v>
+      </c>
+      <c r="I101" s="2" t="str">
+        <f t="shared" si="1"/>
+        <v>available</v>
+      </c>
+    </row>
+    <row r="102" spans="4:9" x14ac:dyDescent="0.2">
+      <c r="D102" t="s">
+        <v>322</v>
+      </c>
+      <c r="E102" t="s">
+        <v>1056</v>
+      </c>
+      <c r="H102" s="6" t="s">
+        <v>966</v>
+      </c>
+      <c r="I102" s="2" t="str">
+        <f t="shared" si="1"/>
+        <v>available</v>
+      </c>
+    </row>
+    <row r="103" spans="4:9" x14ac:dyDescent="0.2">
+      <c r="D103" t="s">
+        <v>326</v>
+      </c>
+      <c r="E103" t="s">
+        <v>1056</v>
+      </c>
+    </row>
+    <row r="104" spans="4:9" x14ac:dyDescent="0.2">
+      <c r="D104" t="s">
+        <v>349</v>
+      </c>
+      <c r="E104" t="s">
+        <v>1056</v>
+      </c>
+    </row>
+    <row r="105" spans="4:9" x14ac:dyDescent="0.2">
+      <c r="D105" t="s">
+        <v>329</v>
+      </c>
+      <c r="E105" t="s">
+        <v>1056</v>
+      </c>
+    </row>
+    <row r="106" spans="4:9" x14ac:dyDescent="0.2">
+      <c r="D106" t="s">
+        <v>306</v>
+      </c>
+      <c r="E106" t="s">
+        <v>1056</v>
+      </c>
+    </row>
+    <row r="107" spans="4:9" x14ac:dyDescent="0.2">
+      <c r="D107" t="s">
+        <v>341</v>
+      </c>
+      <c r="E107" t="s">
+        <v>1056</v>
+      </c>
+    </row>
+    <row r="108" spans="4:9" x14ac:dyDescent="0.2">
+      <c r="D108" t="s">
+        <v>361</v>
+      </c>
+      <c r="E108" t="s">
+        <v>1056</v>
+      </c>
+    </row>
+    <row r="109" spans="4:9" x14ac:dyDescent="0.2">
+      <c r="D109" t="s">
+        <v>357</v>
+      </c>
+      <c r="E109" t="s">
+        <v>1056</v>
+      </c>
+    </row>
+    <row r="110" spans="4:9" x14ac:dyDescent="0.2">
+      <c r="D110" t="s">
+        <v>318</v>
+      </c>
+      <c r="E110" t="s">
+        <v>1056</v>
+      </c>
+    </row>
+    <row r="111" spans="4:9" x14ac:dyDescent="0.2">
+      <c r="D111" t="s">
+        <v>337</v>
+      </c>
+      <c r="E111" t="s">
+        <v>1056</v>
+      </c>
+    </row>
+    <row r="112" spans="4:9" x14ac:dyDescent="0.2">
+      <c r="D112" t="s">
+        <v>364</v>
+      </c>
+      <c r="E112" t="s">
+        <v>1056</v>
+      </c>
+    </row>
+    <row r="113" spans="4:5" x14ac:dyDescent="0.2">
+      <c r="D113" t="s">
+        <v>368</v>
+      </c>
+      <c r="E113" t="s">
+        <v>1056</v>
+      </c>
+    </row>
+    <row r="114" spans="4:5" x14ac:dyDescent="0.2">
+      <c r="D114" t="s">
+        <v>387</v>
+      </c>
+      <c r="E114" t="s">
+        <v>1056</v>
+      </c>
+    </row>
+    <row r="115" spans="4:5" x14ac:dyDescent="0.2">
+      <c r="D115" t="s">
+        <v>375</v>
+      </c>
+      <c r="E115" t="s">
+        <v>1056</v>
+      </c>
+    </row>
+    <row r="116" spans="4:5" x14ac:dyDescent="0.2">
+      <c r="D116" t="s">
+        <v>1026</v>
+      </c>
+      <c r="E116" t="s">
+        <v>1056</v>
+      </c>
+    </row>
+    <row r="117" spans="4:5" x14ac:dyDescent="0.2">
+      <c r="D117" t="s">
+        <v>379</v>
+      </c>
+      <c r="E117" t="s">
+        <v>1056</v>
+      </c>
+    </row>
+    <row r="118" spans="4:5" x14ac:dyDescent="0.2">
+      <c r="D118" t="s">
+        <v>372</v>
+      </c>
+      <c r="E118" t="s">
+        <v>1056</v>
+      </c>
+    </row>
+    <row r="119" spans="4:5" x14ac:dyDescent="0.2">
+      <c r="D119" t="s">
+        <v>391</v>
+      </c>
+      <c r="E119" t="s">
+        <v>1056</v>
+      </c>
+    </row>
+    <row r="120" spans="4:5" x14ac:dyDescent="0.2">
+      <c r="D120" t="s">
+        <v>427</v>
+      </c>
+      <c r="E120" t="s">
+        <v>1056</v>
+      </c>
+    </row>
+    <row r="121" spans="4:5" x14ac:dyDescent="0.2">
+      <c r="D121" t="s">
+        <v>411</v>
+      </c>
+      <c r="E121" t="s">
+        <v>1056</v>
+      </c>
+    </row>
+    <row r="122" spans="4:5" x14ac:dyDescent="0.2">
+      <c r="D122" t="s">
+        <v>395</v>
+      </c>
+      <c r="E122" t="s">
+        <v>1056</v>
+      </c>
+    </row>
+    <row r="123" spans="4:5" x14ac:dyDescent="0.2">
+      <c r="D123" t="s">
+        <v>1027</v>
+      </c>
+      <c r="E123" t="s">
+        <v>1056</v>
+      </c>
+    </row>
+    <row r="124" spans="4:5" x14ac:dyDescent="0.2">
+      <c r="D124" t="s">
+        <v>419</v>
+      </c>
+      <c r="E124" t="s">
+        <v>1056</v>
+      </c>
+    </row>
+    <row r="125" spans="4:5" x14ac:dyDescent="0.2">
+      <c r="D125" t="s">
+        <v>399</v>
+      </c>
+      <c r="E125" t="s">
+        <v>1056</v>
+      </c>
+    </row>
+    <row r="126" spans="4:5" x14ac:dyDescent="0.2">
+      <c r="D126" t="s">
+        <v>407</v>
+      </c>
+      <c r="E126" t="s">
+        <v>1056</v>
+      </c>
+    </row>
+    <row r="127" spans="4:5" x14ac:dyDescent="0.2">
+      <c r="D127" t="s">
+        <v>403</v>
+      </c>
+      <c r="E127" t="s">
+        <v>1056</v>
+      </c>
+    </row>
+    <row r="128" spans="4:5" x14ac:dyDescent="0.2">
+      <c r="D128" t="s">
+        <v>431</v>
+      </c>
+      <c r="E128" t="s">
+        <v>1056</v>
+      </c>
+    </row>
+    <row r="129" spans="4:5" x14ac:dyDescent="0.2">
+      <c r="D129" t="s">
+        <v>438</v>
+      </c>
+      <c r="E129" t="s">
+        <v>1056</v>
+      </c>
+    </row>
+    <row r="130" spans="4:5" x14ac:dyDescent="0.2">
+      <c r="D130" t="s">
+        <v>446</v>
+      </c>
+      <c r="E130" t="s">
+        <v>1056</v>
+      </c>
+    </row>
+    <row r="131" spans="4:5" x14ac:dyDescent="0.2">
+      <c r="D131" t="s">
+        <v>435</v>
+      </c>
+      <c r="E131" t="s">
+        <v>1056</v>
+      </c>
+    </row>
+    <row r="132" spans="4:5" x14ac:dyDescent="0.2">
+      <c r="D132" t="s">
+        <v>442</v>
+      </c>
+      <c r="E132" t="s">
+        <v>1056</v>
+      </c>
+    </row>
+    <row r="133" spans="4:5" x14ac:dyDescent="0.2">
+      <c r="D133" t="s">
+        <v>489</v>
+      </c>
+      <c r="E133" t="s">
+        <v>1056</v>
+      </c>
+    </row>
+    <row r="134" spans="4:5" x14ac:dyDescent="0.2">
+      <c r="D134" t="s">
+        <v>450</v>
+      </c>
+      <c r="E134" t="s">
+        <v>1056</v>
+      </c>
+    </row>
+    <row r="135" spans="4:5" x14ac:dyDescent="0.2">
+      <c r="D135" t="s">
+        <v>462</v>
+      </c>
+      <c r="E135" t="s">
+        <v>1056</v>
+      </c>
+    </row>
+    <row r="136" spans="4:5" x14ac:dyDescent="0.2">
+      <c r="D136" t="s">
+        <v>1028</v>
+      </c>
+      <c r="E136" t="s">
+        <v>1056</v>
+      </c>
+    </row>
+    <row r="137" spans="4:5" x14ac:dyDescent="0.2">
+      <c r="D137" t="s">
+        <v>980</v>
+      </c>
+      <c r="E137" t="s">
+        <v>1056</v>
+      </c>
+    </row>
+    <row r="138" spans="4:5" x14ac:dyDescent="0.2">
+      <c r="D138" t="s">
+        <v>481</v>
+      </c>
+      <c r="E138" t="s">
+        <v>1056</v>
+      </c>
+    </row>
+    <row r="139" spans="4:5" x14ac:dyDescent="0.2">
+      <c r="D139" t="s">
+        <v>454</v>
+      </c>
+      <c r="E139" t="s">
+        <v>1056</v>
+      </c>
+    </row>
+    <row r="140" spans="4:5" x14ac:dyDescent="0.2">
+      <c r="D140" t="s">
+        <v>1029</v>
+      </c>
+      <c r="E140" t="s">
+        <v>1056</v>
+      </c>
+    </row>
+    <row r="141" spans="4:5" x14ac:dyDescent="0.2">
+      <c r="D141" t="s">
+        <v>528</v>
+      </c>
+      <c r="E141" t="s">
+        <v>1056</v>
+      </c>
+    </row>
+    <row r="142" spans="4:5" x14ac:dyDescent="0.2">
+      <c r="D142" t="s">
+        <v>497</v>
+      </c>
+      <c r="E142" t="s">
+        <v>1056</v>
+      </c>
+    </row>
+    <row r="143" spans="4:5" x14ac:dyDescent="0.2">
+      <c r="D143" t="s">
+        <v>516</v>
+      </c>
+      <c r="E143" t="s">
+        <v>1056</v>
+      </c>
+    </row>
+    <row r="144" spans="4:5" x14ac:dyDescent="0.2">
+      <c r="D144" t="s">
+        <v>512</v>
+      </c>
+      <c r="E144" t="s">
+        <v>1056</v>
+      </c>
+    </row>
+    <row r="145" spans="4:5" x14ac:dyDescent="0.2">
+      <c r="D145" t="s">
+        <v>532</v>
+      </c>
+      <c r="E145" t="s">
+        <v>1056</v>
+      </c>
+    </row>
+    <row r="146" spans="4:5" x14ac:dyDescent="0.2">
+      <c r="D146" t="s">
+        <v>505</v>
+      </c>
+      <c r="E146" t="s">
+        <v>1056</v>
+      </c>
+    </row>
+    <row r="147" spans="4:5" x14ac:dyDescent="0.2">
+      <c r="D147" t="s">
+        <v>520</v>
+      </c>
+      <c r="E147" t="s">
+        <v>1056</v>
+      </c>
+    </row>
+    <row r="148" spans="4:5" x14ac:dyDescent="0.2">
+      <c r="D148" t="s">
+        <v>524</v>
+      </c>
+      <c r="E148" t="s">
+        <v>1056</v>
+      </c>
+    </row>
+    <row r="149" spans="4:5" x14ac:dyDescent="0.2">
+      <c r="D149" t="s">
+        <v>1030</v>
+      </c>
+      <c r="E149" t="s">
+        <v>1056</v>
+      </c>
+    </row>
+    <row r="150" spans="4:5" x14ac:dyDescent="0.2">
+      <c r="D150" t="s">
+        <v>555</v>
+      </c>
+      <c r="E150" t="s">
+        <v>1056</v>
+      </c>
+    </row>
+    <row r="151" spans="4:5" x14ac:dyDescent="0.2">
+      <c r="D151" t="s">
+        <v>608</v>
+      </c>
+      <c r="E151" t="s">
+        <v>1056</v>
+      </c>
+    </row>
+    <row r="152" spans="4:5" x14ac:dyDescent="0.2">
+      <c r="D152" t="s">
+        <v>616</v>
+      </c>
+      <c r="E152" t="s">
+        <v>1056</v>
+      </c>
+    </row>
+    <row r="153" spans="4:5" x14ac:dyDescent="0.2">
+      <c r="D153" t="s">
+        <v>604</v>
+      </c>
+      <c r="E153" t="s">
+        <v>1056</v>
+      </c>
+    </row>
+    <row r="154" spans="4:5" x14ac:dyDescent="0.2">
+      <c r="D154" t="s">
+        <v>566</v>
+      </c>
+      <c r="E154" t="s">
+        <v>1056</v>
+      </c>
+    </row>
+    <row r="155" spans="4:5" x14ac:dyDescent="0.2">
+      <c r="D155" t="s">
+        <v>596</v>
+      </c>
+      <c r="E155" t="s">
+        <v>1056</v>
+      </c>
+    </row>
+    <row r="156" spans="4:5" x14ac:dyDescent="0.2">
+      <c r="D156" t="s">
+        <v>1031</v>
+      </c>
+      <c r="E156" t="s">
+        <v>1056</v>
+      </c>
+    </row>
+    <row r="157" spans="4:5" x14ac:dyDescent="0.2">
+      <c r="D157" t="s">
+        <v>585</v>
+      </c>
+      <c r="E157" t="s">
+        <v>1056</v>
+      </c>
+    </row>
+    <row r="158" spans="4:5" x14ac:dyDescent="0.2">
+      <c r="D158" t="s">
+        <v>589</v>
+      </c>
+      <c r="E158" t="s">
+        <v>1056</v>
+      </c>
+    </row>
+    <row r="159" spans="4:5" x14ac:dyDescent="0.2">
+      <c r="D159" t="s">
+        <v>600</v>
+      </c>
+      <c r="E159" t="s">
+        <v>1056</v>
+      </c>
+    </row>
+    <row r="160" spans="4:5" x14ac:dyDescent="0.2">
+      <c r="D160" t="s">
+        <v>963</v>
+      </c>
+      <c r="E160" t="s">
+        <v>1056</v>
+      </c>
+    </row>
+    <row r="161" spans="4:5" x14ac:dyDescent="0.2">
+      <c r="D161" t="s">
+        <v>612</v>
+      </c>
+      <c r="E161" t="s">
+        <v>1056</v>
+      </c>
+    </row>
+    <row r="162" spans="4:5" x14ac:dyDescent="0.2">
+      <c r="D162" t="s">
+        <v>1032</v>
+      </c>
+      <c r="E162" t="s">
+        <v>1056</v>
+      </c>
+    </row>
+    <row r="163" spans="4:5" x14ac:dyDescent="0.2">
+      <c r="D163" t="s">
+        <v>1033</v>
+      </c>
+      <c r="E163" t="s">
+        <v>1056</v>
+      </c>
+    </row>
+    <row r="164" spans="4:5" x14ac:dyDescent="0.2">
+      <c r="D164" t="s">
+        <v>540</v>
+      </c>
+      <c r="E164" t="s">
+        <v>1056</v>
+      </c>
+    </row>
+    <row r="165" spans="4:5" x14ac:dyDescent="0.2">
+      <c r="D165" t="s">
+        <v>574</v>
+      </c>
+      <c r="E165" t="s">
+        <v>1056</v>
+      </c>
+    </row>
+    <row r="166" spans="4:5" x14ac:dyDescent="0.2">
+      <c r="D166" t="s">
+        <v>547</v>
+      </c>
+      <c r="E166" t="s">
+        <v>1056</v>
+      </c>
+    </row>
+    <row r="167" spans="4:5" x14ac:dyDescent="0.2">
+      <c r="D167" t="s">
+        <v>593</v>
+      </c>
+      <c r="E167" t="s">
+        <v>1056</v>
+      </c>
+    </row>
+    <row r="168" spans="4:5" x14ac:dyDescent="0.2">
+      <c r="D168" t="s">
+        <v>536</v>
+      </c>
+      <c r="E168" t="s">
+        <v>1056</v>
+      </c>
+    </row>
+    <row r="169" spans="4:5" x14ac:dyDescent="0.2">
+      <c r="D169" t="s">
+        <v>620</v>
+      </c>
+      <c r="E169" t="s">
+        <v>1056</v>
+      </c>
+    </row>
+    <row r="170" spans="4:5" x14ac:dyDescent="0.2">
+      <c r="D170" t="s">
+        <v>624</v>
+      </c>
+      <c r="E170" t="s">
+        <v>1056</v>
+      </c>
+    </row>
+    <row r="171" spans="4:5" x14ac:dyDescent="0.2">
+      <c r="D171" t="s">
+        <v>660</v>
+      </c>
+      <c r="E171" t="s">
+        <v>1056</v>
+      </c>
+    </row>
+    <row r="172" spans="4:5" x14ac:dyDescent="0.2">
+      <c r="D172" t="s">
+        <v>656</v>
+      </c>
+      <c r="E172" t="s">
+        <v>1056</v>
+      </c>
+    </row>
+    <row r="173" spans="4:5" x14ac:dyDescent="0.2">
+      <c r="D173" t="s">
+        <v>1034</v>
+      </c>
+      <c r="E173" t="s">
+        <v>1056</v>
+      </c>
+    </row>
+    <row r="174" spans="4:5" x14ac:dyDescent="0.2">
+      <c r="D174" t="s">
+        <v>1035</v>
+      </c>
+      <c r="E174" t="s">
+        <v>1056</v>
+      </c>
+    </row>
+    <row r="175" spans="4:5" x14ac:dyDescent="0.2">
+      <c r="D175" t="s">
+        <v>628</v>
+      </c>
+      <c r="E175" t="s">
+        <v>1056</v>
+      </c>
+    </row>
+    <row r="176" spans="4:5" x14ac:dyDescent="0.2">
+      <c r="D176" t="s">
+        <v>666</v>
+      </c>
+      <c r="E176" t="s">
+        <v>1056</v>
+      </c>
+    </row>
+    <row r="177" spans="4:5" x14ac:dyDescent="0.2">
+      <c r="D177" t="s">
+        <v>644</v>
+      </c>
+      <c r="E177" t="s">
+        <v>1056</v>
+      </c>
+    </row>
+    <row r="178" spans="4:5" x14ac:dyDescent="0.2">
+      <c r="D178" t="s">
+        <v>1036</v>
+      </c>
+      <c r="E178" t="s">
+        <v>1056</v>
+      </c>
+    </row>
+    <row r="179" spans="4:5" x14ac:dyDescent="0.2">
+      <c r="D179" t="s">
+        <v>640</v>
+      </c>
+      <c r="E179" t="s">
+        <v>1056</v>
+      </c>
+    </row>
+    <row r="180" spans="4:5" x14ac:dyDescent="0.2">
+      <c r="D180" t="s">
+        <v>663</v>
+      </c>
+      <c r="E180" t="s">
+        <v>1056</v>
+      </c>
+    </row>
+    <row r="181" spans="4:5" x14ac:dyDescent="0.2">
+      <c r="D181" t="s">
+        <v>636</v>
+      </c>
+      <c r="E181" t="s">
+        <v>1056</v>
+      </c>
+    </row>
+    <row r="182" spans="4:5" x14ac:dyDescent="0.2">
+      <c r="D182" t="s">
+        <v>1037</v>
+      </c>
+      <c r="E182" t="s">
+        <v>1056</v>
+      </c>
+    </row>
+    <row r="183" spans="4:5" x14ac:dyDescent="0.2">
+      <c r="D183" t="s">
+        <v>562</v>
+      </c>
+      <c r="E183" t="s">
+        <v>1056</v>
+      </c>
+    </row>
+    <row r="184" spans="4:5" x14ac:dyDescent="0.2">
+      <c r="D184" t="s">
+        <v>1038</v>
+      </c>
+      <c r="E184" t="s">
+        <v>1056</v>
+      </c>
+    </row>
+    <row r="185" spans="4:5" x14ac:dyDescent="0.2">
+      <c r="D185" t="s">
+        <v>652</v>
+      </c>
+      <c r="E185" t="s">
+        <v>1056</v>
+      </c>
+    </row>
+    <row r="186" spans="4:5" x14ac:dyDescent="0.2">
+      <c r="D186" t="s">
+        <v>670</v>
+      </c>
+      <c r="E186" t="s">
+        <v>1056</v>
+      </c>
+    </row>
+    <row r="187" spans="4:5" x14ac:dyDescent="0.2">
+      <c r="D187" t="s">
+        <v>693</v>
+      </c>
+      <c r="E187" t="s">
+        <v>1056</v>
+      </c>
+    </row>
+    <row r="188" spans="4:5" x14ac:dyDescent="0.2">
+      <c r="D188" t="s">
+        <v>720</v>
+      </c>
+      <c r="E188" t="s">
+        <v>1056</v>
+      </c>
+    </row>
+    <row r="189" spans="4:5" x14ac:dyDescent="0.2">
+      <c r="D189" t="s">
+        <v>1039</v>
+      </c>
+      <c r="E189" t="s">
+        <v>1056</v>
+      </c>
+    </row>
+    <row r="190" spans="4:5" x14ac:dyDescent="0.2">
+      <c r="D190" t="s">
+        <v>673</v>
+      </c>
+      <c r="E190" t="s">
+        <v>1056</v>
+      </c>
+    </row>
+    <row r="191" spans="4:5" x14ac:dyDescent="0.2">
+      <c r="D191" t="s">
+        <v>685</v>
+      </c>
+      <c r="E191" t="s">
+        <v>1056</v>
+      </c>
+    </row>
+    <row r="192" spans="4:5" x14ac:dyDescent="0.2">
+      <c r="D192" t="s">
+        <v>724</v>
+      </c>
+      <c r="E192" t="s">
+        <v>1056</v>
+      </c>
+    </row>
+    <row r="193" spans="4:5" x14ac:dyDescent="0.2">
+      <c r="D193" t="s">
+        <v>677</v>
+      </c>
+      <c r="E193" t="s">
+        <v>1056</v>
+      </c>
+    </row>
+    <row r="194" spans="4:5" x14ac:dyDescent="0.2">
+      <c r="D194" t="s">
+        <v>1040</v>
+      </c>
+      <c r="E194" t="s">
+        <v>1056</v>
+      </c>
+    </row>
+    <row r="195" spans="4:5" x14ac:dyDescent="0.2">
+      <c r="D195" t="s">
+        <v>1041</v>
+      </c>
+      <c r="E195" t="s">
+        <v>1056</v>
+      </c>
+    </row>
+    <row r="196" spans="4:5" x14ac:dyDescent="0.2">
+      <c r="D196" t="s">
+        <v>697</v>
+      </c>
+      <c r="E196" t="s">
+        <v>1056</v>
+      </c>
+    </row>
+    <row r="197" spans="4:5" x14ac:dyDescent="0.2">
+      <c r="D197" t="s">
+        <v>716</v>
+      </c>
+      <c r="E197" t="s">
+        <v>1056</v>
+      </c>
+    </row>
+    <row r="198" spans="4:5" x14ac:dyDescent="0.2">
+      <c r="D198" t="s">
+        <v>708</v>
+      </c>
+      <c r="E198" t="s">
+        <v>1056</v>
+      </c>
+    </row>
+    <row r="199" spans="4:5" x14ac:dyDescent="0.2">
+      <c r="D199" t="s">
+        <v>728</v>
+      </c>
+      <c r="E199" t="s">
+        <v>1056</v>
+      </c>
+    </row>
+    <row r="200" spans="4:5" x14ac:dyDescent="0.2">
+      <c r="D200" t="s">
+        <v>732</v>
+      </c>
+      <c r="E200" t="s">
+        <v>1056</v>
+      </c>
+    </row>
+    <row r="201" spans="4:5" x14ac:dyDescent="0.2">
+      <c r="D201" t="s">
+        <v>736</v>
+      </c>
+      <c r="E201" t="s">
+        <v>1056</v>
+      </c>
+    </row>
+    <row r="202" spans="4:5" x14ac:dyDescent="0.2">
+      <c r="D202" t="s">
+        <v>1042</v>
+      </c>
+      <c r="E202" t="s">
+        <v>1056</v>
+      </c>
+    </row>
+    <row r="203" spans="4:5" x14ac:dyDescent="0.2">
+      <c r="D203" t="s">
+        <v>748</v>
+      </c>
+      <c r="E203" t="s">
+        <v>1056</v>
+      </c>
+    </row>
+    <row r="204" spans="4:5" x14ac:dyDescent="0.2">
+      <c r="D204" t="s">
+        <v>1043</v>
+      </c>
+      <c r="E204" t="s">
+        <v>1056</v>
+      </c>
+    </row>
+    <row r="205" spans="4:5" x14ac:dyDescent="0.2">
+      <c r="D205" t="s">
+        <v>469</v>
+      </c>
+      <c r="E205" t="s">
+        <v>1056</v>
+      </c>
+    </row>
+    <row r="206" spans="4:5" x14ac:dyDescent="0.2">
+      <c r="D206" t="s">
+        <v>501</v>
+      </c>
+      <c r="E206" t="s">
+        <v>1056</v>
+      </c>
+    </row>
+    <row r="207" spans="4:5" x14ac:dyDescent="0.2">
+      <c r="D207" t="s">
+        <v>701</v>
+      </c>
+      <c r="E207" t="s">
+        <v>1056</v>
+      </c>
+    </row>
+    <row r="208" spans="4:5" x14ac:dyDescent="0.2">
+      <c r="D208" t="s">
+        <v>927</v>
+      </c>
+      <c r="E208" t="s">
+        <v>1056</v>
+      </c>
+    </row>
+    <row r="209" spans="4:5" x14ac:dyDescent="0.2">
+      <c r="D209" t="s">
+        <v>955</v>
+      </c>
+      <c r="E209" t="s">
+        <v>1056</v>
+      </c>
+    </row>
+    <row r="210" spans="4:5" x14ac:dyDescent="0.2">
+      <c r="D210" t="s">
+        <v>796</v>
+      </c>
+      <c r="E210" t="s">
+        <v>1056</v>
+      </c>
+    </row>
+    <row r="211" spans="4:5" x14ac:dyDescent="0.2">
+      <c r="D211" t="s">
+        <v>816</v>
+      </c>
+      <c r="E211" t="s">
+        <v>1056</v>
+      </c>
+    </row>
+    <row r="212" spans="4:5" x14ac:dyDescent="0.2">
+      <c r="D212" t="s">
+        <v>752</v>
+      </c>
+      <c r="E212" t="s">
+        <v>1056</v>
+      </c>
+    </row>
+    <row r="213" spans="4:5" x14ac:dyDescent="0.2">
+      <c r="D213" t="s">
+        <v>800</v>
+      </c>
+      <c r="E213" t="s">
+        <v>1056</v>
+      </c>
+    </row>
+    <row r="214" spans="4:5" x14ac:dyDescent="0.2">
+      <c r="D214" t="s">
+        <v>740</v>
+      </c>
+      <c r="E214" t="s">
+        <v>1056</v>
+      </c>
+    </row>
+    <row r="215" spans="4:5" x14ac:dyDescent="0.2">
+      <c r="D215" t="s">
+        <v>760</v>
+      </c>
+      <c r="E215" t="s">
+        <v>1056</v>
+      </c>
+    </row>
+    <row r="216" spans="4:5" x14ac:dyDescent="0.2">
+      <c r="D216" t="s">
+        <v>792</v>
+      </c>
+      <c r="E216" t="s">
+        <v>1056</v>
+      </c>
+    </row>
+    <row r="217" spans="4:5" x14ac:dyDescent="0.2">
+      <c r="D217" t="s">
+        <v>772</v>
+      </c>
+      <c r="E217" t="s">
+        <v>1056</v>
+      </c>
+    </row>
+    <row r="218" spans="4:5" x14ac:dyDescent="0.2">
+      <c r="D218" t="s">
+        <v>788</v>
+      </c>
+      <c r="E218" t="s">
+        <v>1056</v>
+      </c>
+    </row>
+    <row r="219" spans="4:5" x14ac:dyDescent="0.2">
+      <c r="D219" t="s">
+        <v>780</v>
+      </c>
+      <c r="E219" t="s">
+        <v>1056</v>
+      </c>
+    </row>
+    <row r="220" spans="4:5" x14ac:dyDescent="0.2">
+      <c r="D220" t="s">
+        <v>756</v>
+      </c>
+      <c r="E220" t="s">
+        <v>1056</v>
+      </c>
+    </row>
+    <row r="221" spans="4:5" x14ac:dyDescent="0.2">
+      <c r="D221" t="s">
+        <v>804</v>
+      </c>
+      <c r="E221" t="s">
+        <v>1056</v>
+      </c>
+    </row>
+    <row r="222" spans="4:5" x14ac:dyDescent="0.2">
+      <c r="D222" t="s">
+        <v>966</v>
+      </c>
+      <c r="E222" t="s">
+        <v>1056</v>
+      </c>
+    </row>
+    <row r="223" spans="4:5" x14ac:dyDescent="0.2">
+      <c r="D223" t="s">
+        <v>353</v>
+      </c>
+      <c r="E223" t="s">
+        <v>1056</v>
+      </c>
+    </row>
+    <row r="224" spans="4:5" x14ac:dyDescent="0.2">
+      <c r="D224" t="s">
+        <v>812</v>
+      </c>
+      <c r="E224" t="s">
+        <v>1056</v>
+      </c>
+    </row>
+    <row r="225" spans="4:5" x14ac:dyDescent="0.2">
+      <c r="D225" t="s">
+        <v>266</v>
+      </c>
+      <c r="E225" t="s">
+        <v>1056</v>
+      </c>
+    </row>
+    <row r="226" spans="4:5" x14ac:dyDescent="0.2">
+      <c r="D226" t="s">
+        <v>509</v>
+      </c>
+      <c r="E226" t="s">
+        <v>1056</v>
+      </c>
+    </row>
+    <row r="227" spans="4:5" x14ac:dyDescent="0.2">
+      <c r="D227" t="s">
+        <v>1044</v>
+      </c>
+      <c r="E227" t="s">
+        <v>1056</v>
+      </c>
+    </row>
+    <row r="228" spans="4:5" x14ac:dyDescent="0.2">
+      <c r="D228" t="s">
+        <v>808</v>
+      </c>
+      <c r="E228" t="s">
+        <v>1056</v>
+      </c>
+    </row>
+    <row r="229" spans="4:5" x14ac:dyDescent="0.2">
+      <c r="D229" t="s">
+        <v>784</v>
+      </c>
+      <c r="E229" t="s">
+        <v>1056</v>
+      </c>
+    </row>
+    <row r="230" spans="4:5" x14ac:dyDescent="0.2">
+      <c r="D230" t="s">
+        <v>768</v>
+      </c>
+      <c r="E230" t="s">
+        <v>1056</v>
+      </c>
+    </row>
+    <row r="231" spans="4:5" x14ac:dyDescent="0.2">
+      <c r="D231" t="s">
+        <v>170</v>
+      </c>
+      <c r="E231" t="s">
+        <v>1056</v>
+      </c>
+    </row>
+    <row r="232" spans="4:5" x14ac:dyDescent="0.2">
+      <c r="D232" t="s">
+        <v>1045</v>
+      </c>
+      <c r="E232" t="s">
+        <v>1056</v>
+      </c>
+    </row>
+    <row r="233" spans="4:5" x14ac:dyDescent="0.2">
+      <c r="D233" t="s">
+        <v>1046</v>
+      </c>
+      <c r="E233" t="s">
+        <v>1056</v>
+      </c>
+    </row>
+    <row r="234" spans="4:5" x14ac:dyDescent="0.2">
+      <c r="D234" t="s">
+        <v>855</v>
+      </c>
+      <c r="E234" t="s">
+        <v>1056</v>
+      </c>
+    </row>
+    <row r="235" spans="4:5" x14ac:dyDescent="0.2">
+      <c r="D235" t="s">
+        <v>1047</v>
+      </c>
+      <c r="E235" t="s">
+        <v>1056</v>
+      </c>
+    </row>
+    <row r="236" spans="4:5" x14ac:dyDescent="0.2">
+      <c r="D236" t="s">
+        <v>851</v>
+      </c>
+      <c r="E236" t="s">
+        <v>1056</v>
+      </c>
+    </row>
+    <row r="237" spans="4:5" x14ac:dyDescent="0.2">
+      <c r="D237" t="s">
+        <v>863</v>
+      </c>
+      <c r="E237" t="s">
+        <v>1056</v>
+      </c>
+    </row>
+    <row r="238" spans="4:5" x14ac:dyDescent="0.2">
+      <c r="D238" t="s">
+        <v>847</v>
+      </c>
+      <c r="E238" t="s">
+        <v>1056</v>
+      </c>
+    </row>
+    <row r="239" spans="4:5" x14ac:dyDescent="0.2">
+      <c r="D239" t="s">
+        <v>859</v>
+      </c>
+      <c r="E239" t="s">
+        <v>1056</v>
+      </c>
+    </row>
+    <row r="240" spans="4:5" x14ac:dyDescent="0.2">
+      <c r="D240" t="s">
+        <v>875</v>
+      </c>
+      <c r="E240" t="s">
+        <v>1056</v>
+      </c>
+    </row>
+    <row r="241" spans="4:5" x14ac:dyDescent="0.2">
+      <c r="D241" t="s">
+        <v>883</v>
+      </c>
+      <c r="E241" t="s">
+        <v>1056</v>
+      </c>
+    </row>
+    <row r="242" spans="4:5" x14ac:dyDescent="0.2">
+      <c r="D242" t="s">
+        <v>871</v>
+      </c>
+      <c r="E242" t="s">
+        <v>1056</v>
+      </c>
+    </row>
+    <row r="243" spans="4:5" x14ac:dyDescent="0.2">
+      <c r="D243" t="s">
+        <v>879</v>
+      </c>
+      <c r="E243" t="s">
+        <v>1056</v>
+      </c>
+    </row>
+    <row r="244" spans="4:5" x14ac:dyDescent="0.2">
+      <c r="D244" t="s">
+        <v>867</v>
+      </c>
+      <c r="E244" t="s">
+        <v>1056</v>
+      </c>
+    </row>
+    <row r="245" spans="4:5" x14ac:dyDescent="0.2">
+      <c r="D245" t="s">
+        <v>1048</v>
+      </c>
+      <c r="E245" t="s">
+        <v>1056</v>
+      </c>
+    </row>
+    <row r="246" spans="4:5" x14ac:dyDescent="0.2">
+      <c r="D246" t="s">
+        <v>887</v>
+      </c>
+      <c r="E246" t="s">
+        <v>1056</v>
+      </c>
+    </row>
+    <row r="247" spans="4:5" x14ac:dyDescent="0.2">
+      <c r="D247" t="s">
+        <v>1049</v>
+      </c>
+      <c r="E247" t="s">
+        <v>1056</v>
+      </c>
+    </row>
+    <row r="248" spans="4:5" x14ac:dyDescent="0.2">
+      <c r="D248" t="s">
+        <v>1050</v>
+      </c>
+      <c r="E248" t="s">
+        <v>1056</v>
+      </c>
+    </row>
+    <row r="249" spans="4:5" x14ac:dyDescent="0.2">
+      <c r="D249" t="s">
+        <v>903</v>
+      </c>
+      <c r="E249" t="s">
+        <v>1056</v>
+      </c>
+    </row>
+    <row r="250" spans="4:5" x14ac:dyDescent="0.2">
+      <c r="D250" t="s">
+        <v>899</v>
+      </c>
+      <c r="E250" t="s">
+        <v>1056</v>
+      </c>
+    </row>
+    <row r="251" spans="4:5" x14ac:dyDescent="0.2">
+      <c r="D251" t="s">
+        <v>1051</v>
+      </c>
+      <c r="E251" t="s">
+        <v>1056</v>
+      </c>
+    </row>
+    <row r="252" spans="4:5" x14ac:dyDescent="0.2">
+      <c r="D252" t="s">
+        <v>1052</v>
+      </c>
+      <c r="E252" t="s">
+        <v>1056</v>
+      </c>
+    </row>
+    <row r="253" spans="4:5" x14ac:dyDescent="0.2">
+      <c r="D253" t="s">
+        <v>915</v>
+      </c>
+      <c r="E253" t="s">
+        <v>1056</v>
+      </c>
+    </row>
+    <row r="254" spans="4:5" x14ac:dyDescent="0.2">
+      <c r="D254" t="s">
+        <v>913</v>
+      </c>
+      <c r="E254" t="s">
+        <v>1056</v>
+      </c>
+    </row>
+    <row r="255" spans="4:5" x14ac:dyDescent="0.2">
+      <c r="D255" t="s">
+        <v>919</v>
+      </c>
+      <c r="E255" t="s">
+        <v>1056</v>
+      </c>
+    </row>
+    <row r="256" spans="4:5" x14ac:dyDescent="0.2">
+      <c r="D256" t="s">
+        <v>947</v>
+      </c>
+      <c r="E256" t="s">
+        <v>1056</v>
+      </c>
+    </row>
+    <row r="257" spans="4:5" x14ac:dyDescent="0.2">
+      <c r="D257" t="s">
+        <v>1053</v>
+      </c>
+      <c r="E257" t="s">
+        <v>1056</v>
+      </c>
+    </row>
+    <row r="258" spans="4:5" x14ac:dyDescent="0.2">
+      <c r="D258" t="s">
+        <v>1054</v>
+      </c>
+      <c r="E258" t="s">
+        <v>1056</v>
+      </c>
+    </row>
+    <row r="259" spans="4:5" x14ac:dyDescent="0.2">
+      <c r="D259" t="s">
+        <v>951</v>
+      </c>
+      <c r="E259" t="s">
+        <v>1056</v>
+      </c>
+    </row>
+    <row r="260" spans="4:5" x14ac:dyDescent="0.2">
+      <c r="D260" t="s">
+        <v>1055</v>
+      </c>
+      <c r="E260" t="s">
+        <v>1056</v>
+      </c>
+    </row>
+    <row r="261" spans="4:5" x14ac:dyDescent="0.2">
+      <c r="D261" t="s">
+        <v>959</v>
+      </c>
+      <c r="E261" t="s">
+        <v>1056</v>
+      </c>
+    </row>
+    <row r="262" spans="4:5" x14ac:dyDescent="0.2">
+      <c r="D262" t="s">
+        <v>970</v>
+      </c>
+      <c r="E262" t="s">
+        <v>1056</v>
+      </c>
+    </row>
+    <row r="263" spans="4:5" x14ac:dyDescent="0.2">
+      <c r="D263" t="s">
+        <v>974</v>
+      </c>
+      <c r="E263" t="s">
+        <v>1056</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5DA00403-89E7-9540-8B57-52125BDF6C1E}">
+  <dimension ref="A1:A32"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E40" sqref="E40"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="19" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="19" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>1057</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>1020</v>
+      </c>
+    </row>
+    <row r="10" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="11" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>322</v>
+      </c>
+    </row>
+    <row r="12" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>391</v>
+      </c>
+    </row>
+    <row r="13" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>395</v>
+      </c>
+    </row>
+    <row r="14" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>489</v>
+      </c>
+    </row>
+    <row r="15" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>616</v>
+      </c>
+    </row>
+    <row r="16" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>612</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
+        <v>640</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
+        <v>670</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
+        <v>673</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A20" t="s">
+        <v>677</v>
+      </c>
+    </row>
+    <row r="21" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A21" t="s">
+        <v>1040</v>
+      </c>
+    </row>
+    <row r="22" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A22" t="s">
+        <v>697</v>
+      </c>
+    </row>
+    <row r="23" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A23" t="s">
+        <v>728</v>
+      </c>
+    </row>
+    <row r="24" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A24" t="s">
+        <v>736</v>
+      </c>
+    </row>
+    <row r="25" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A25" t="s">
+        <v>1042</v>
+      </c>
+    </row>
+    <row r="26" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A26" t="s">
+        <v>752</v>
+      </c>
+    </row>
+    <row r="27" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A27" t="s">
+        <v>966</v>
+      </c>
+    </row>
+    <row r="28" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A28" t="s">
+        <v>509</v>
+      </c>
+    </row>
+    <row r="29" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A29" t="s">
+        <v>879</v>
+      </c>
+    </row>
+    <row r="30" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A30" t="s">
+        <v>899</v>
+      </c>
+    </row>
+    <row r="31" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A31" t="s">
+        <v>1051</v>
+      </c>
+    </row>
+    <row r="32" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A32" t="s">
+        <v>915</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6FB38D6F-6909-4E4F-8E9D-78822FC7651C}">
+  <dimension ref="A1:A34"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:A34"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>1057</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>1051</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="10" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>1020</v>
+      </c>
+    </row>
+    <row r="11" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="12" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>322</v>
+      </c>
+    </row>
+    <row r="13" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>391</v>
+      </c>
+    </row>
+    <row r="14" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>395</v>
+      </c>
+    </row>
+    <row r="15" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>411</v>
+      </c>
+    </row>
+    <row r="16" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>489</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
+        <v>509</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
+        <v>612</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
+        <v>616</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A20" t="s">
+        <v>640</v>
+      </c>
+    </row>
+    <row r="21" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A21" t="s">
+        <v>670</v>
+      </c>
+    </row>
+    <row r="22" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A22" t="s">
+        <v>673</v>
+      </c>
+    </row>
+    <row r="23" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A23" t="s">
+        <v>677</v>
+      </c>
+    </row>
+    <row r="24" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A24" t="s">
+        <v>1040</v>
+      </c>
+    </row>
+    <row r="25" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A25" t="s">
+        <v>697</v>
+      </c>
+    </row>
+    <row r="26" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A26" t="s">
+        <v>728</v>
+      </c>
+    </row>
+    <row r="27" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A27" t="s">
+        <v>736</v>
+      </c>
+    </row>
+    <row r="28" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A28" t="s">
+        <v>1042</v>
+      </c>
+    </row>
+    <row r="29" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A29" t="s">
+        <v>752</v>
+      </c>
+    </row>
+    <row r="30" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A30" t="s">
+        <v>851</v>
+      </c>
+    </row>
+    <row r="31" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A31" t="s">
+        <v>879</v>
+      </c>
+    </row>
+    <row r="32" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A32" t="s">
+        <v>899</v>
+      </c>
+    </row>
+    <row r="33" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A33" t="s">
+        <v>915</v>
+      </c>
+    </row>
+    <row r="34" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A34" t="s">
+        <v>966</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{21159615-A442-4148-8A2C-81577B6C18D5}">
+  <dimension ref="A1:A20"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:A20"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>1057</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>1020</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>391</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>395</v>
+      </c>
+    </row>
+    <row r="10" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>612</v>
+      </c>
+    </row>
+    <row r="11" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>616</v>
+      </c>
+    </row>
+    <row r="12" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>677</v>
+      </c>
+    </row>
+    <row r="13" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>1040</v>
+      </c>
+    </row>
+    <row r="14" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>697</v>
+      </c>
+    </row>
+    <row r="15" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>736</v>
+      </c>
+    </row>
+    <row r="16" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>1042</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
+        <v>851</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
+        <v>879</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
+        <v>915</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A20" t="s">
+        <v>966</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>